<commit_message>
Fix elements childs structure when client is an entity.
</commit_message>
<xml_diff>
--- a/resources/EIF0590-20210531.xlsx
+++ b/resources/EIF0590-20210531.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="V2.5" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'V2.5'!$G$7:$G$352</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -6626,7 +6629,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -6648,7 +6650,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -6656,7 +6657,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -6664,10 +6664,9 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6678,6 +6677,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF003366"/>
         <bgColor rgb="FF333399"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -6752,7 +6757,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6801,6 +6806,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6826,7 +6847,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1390320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6857,16 +6878,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CB352"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5:CB5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.15"/>
@@ -6878,7 +6899,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="80.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="41.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="38.86"/>
@@ -6948,7 +6969,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="81" style="1" width="11.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7002,7 +7023,7 @@
       <c r="AZ1" s="4"/>
       <c r="BA1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -7056,7 +7077,7 @@
       <c r="AZ2" s="4"/>
       <c r="BA2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7642,7 +7663,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>1</v>
       </c>
@@ -7761,7 +7782,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>2</v>
       </c>
@@ -7904,7 +7925,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>3</v>
       </c>
@@ -8070,7 +8091,7 @@
         <v>44319</v>
       </c>
       <c r="F11" s="11" t="n">
-        <v>0.436805555555555</v>
+        <v>0.436805555555556</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>141</v>
@@ -8136,7 +8157,7 @@
         <v>44319</v>
       </c>
       <c r="AM11" s="11" t="n">
-        <v>0.436805555555555</v>
+        <v>0.436805555555556</v>
       </c>
       <c r="AN11" s="1" t="s">
         <v>104</v>
@@ -8184,7 +8205,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>5</v>
       </c>
@@ -8437,7 +8458,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>7</v>
       </c>
@@ -8553,7 +8574,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>8</v>
       </c>
@@ -8666,7 +8687,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>9</v>
       </c>
@@ -8812,7 +8833,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>10</v>
       </c>
@@ -8925,7 +8946,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>11</v>
       </c>
@@ -9068,7 +9089,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>12</v>
       </c>
@@ -9184,117 +9205,117 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="n">
         <v>13</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="1" t="n">
+      <c r="B20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="13" t="n">
         <v>44319</v>
       </c>
-      <c r="F20" s="11" t="n">
+      <c r="F20" s="14" t="n">
         <v>0.636111111111111</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P20" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="R20" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="S20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="T20" s="1" t="n">
+      <c r="T20" s="12" t="n">
         <v>358351</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="W20" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="X20" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="Y20" s="1" t="s">
+      <c r="Y20" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="Z20" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AB20" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="AE20" s="1" t="s">
+      <c r="AE20" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AF20" s="1" t="s">
+      <c r="AF20" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AG20" s="1" t="s">
+      <c r="AG20" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AI20" s="1" t="n">
+      <c r="AI20" s="12" t="n">
         <v>2500000</v>
       </c>
-      <c r="AJ20" s="3" t="n">
+      <c r="AJ20" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="AK20" s="1" t="s">
+      <c r="AK20" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="AL20" s="2" t="n">
+      <c r="AL20" s="13" t="n">
         <v>44319</v>
       </c>
-      <c r="AM20" s="11" t="n">
+      <c r="AM20" s="14" t="n">
         <v>0.636111111111111</v>
       </c>
-      <c r="AN20" s="1" t="s">
+      <c r="AN20" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="AP20" s="1" t="s">
+      <c r="AP20" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="AQ20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BJ20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BZ20" s="1" t="n">
+      <c r="AQ20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="BJ20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="BZ20" s="12" t="n">
         <v>140588842</v>
       </c>
-      <c r="CA20" s="1" t="n">
+      <c r="CA20" s="12" t="n">
         <v>263933</v>
       </c>
-      <c r="CB20" s="1" t="s">
+      <c r="CB20" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>14</v>
       </c>
@@ -9407,7 +9428,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>15</v>
       </c>
@@ -9520,7 +9541,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>16</v>
       </c>
@@ -9633,7 +9654,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>17</v>
       </c>
@@ -9746,7 +9767,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>18</v>
       </c>
@@ -9889,7 +9910,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>19</v>
       </c>
@@ -10404,7 +10425,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>23</v>
       </c>
@@ -10520,7 +10541,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>24</v>
       </c>
@@ -10636,7 +10657,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>25</v>
       </c>
@@ -10770,7 +10791,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>26</v>
       </c>
@@ -11026,7 +11047,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>28</v>
       </c>
@@ -11139,7 +11160,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>29</v>
       </c>
@@ -11282,7 +11303,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>30</v>
       </c>
@@ -11398,7 +11419,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>31</v>
       </c>
@@ -11514,7 +11535,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>32</v>
       </c>
@@ -11630,7 +11651,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>33</v>
       </c>
@@ -11743,7 +11764,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>34</v>
       </c>
@@ -11760,7 +11781,7 @@
         <v>44320</v>
       </c>
       <c r="F41" s="11" t="n">
-        <v>0.674305555555556</v>
+        <v>0.674305555555555</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>85</v>
@@ -11832,7 +11853,7 @@
         <v>44320</v>
       </c>
       <c r="AM41" s="11" t="n">
-        <v>0.674305555555556</v>
+        <v>0.674305555555555</v>
       </c>
       <c r="AN41" s="1" t="s">
         <v>104</v>
@@ -11889,7 +11910,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>35</v>
       </c>
@@ -12002,7 +12023,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>36</v>
       </c>
@@ -12115,7 +12136,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>37</v>
       </c>
@@ -12228,7 +12249,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>38</v>
       </c>
@@ -12347,7 +12368,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>39</v>
       </c>
@@ -12460,7 +12481,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>40</v>
       </c>
@@ -12573,7 +12594,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>41</v>
       </c>
@@ -12692,7 +12713,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>42</v>
       </c>
@@ -12921,7 +12942,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>44</v>
       </c>
@@ -13034,7 +13055,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>45</v>
       </c>
@@ -13177,7 +13198,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>46</v>
       </c>
@@ -13290,7 +13311,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>47</v>
       </c>
@@ -13427,7 +13448,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>48</v>
       </c>
@@ -13570,7 +13591,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>49</v>
       </c>
@@ -13683,7 +13704,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>50</v>
       </c>
@@ -13796,7 +13817,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>51</v>
       </c>
@@ -13939,7 +13960,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>52</v>
       </c>
@@ -14052,7 +14073,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>53</v>
       </c>
@@ -14168,7 +14189,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>54</v>
       </c>
@@ -14290,7 +14311,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <v>55</v>
       </c>
@@ -14406,7 +14427,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>56</v>
       </c>
@@ -14519,7 +14540,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>57</v>
       </c>
@@ -14635,7 +14656,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <v>58</v>
       </c>
@@ -14745,7 +14766,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <v>59</v>
       </c>
@@ -14858,7 +14879,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>60</v>
       </c>
@@ -15248,7 +15269,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <v>63</v>
       </c>
@@ -16150,7 +16171,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
         <v>70</v>
       </c>
@@ -16266,7 +16287,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
         <v>71</v>
       </c>
@@ -16283,7 +16304,7 @@
         <v>44322</v>
       </c>
       <c r="F78" s="11" t="n">
-        <v>0.480555555555556</v>
+        <v>0.480555555555555</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>85</v>
@@ -16352,7 +16373,7 @@
         <v>44322</v>
       </c>
       <c r="AM78" s="11" t="n">
-        <v>0.480555555555556</v>
+        <v>0.480555555555555</v>
       </c>
       <c r="AN78" s="1" t="s">
         <v>104</v>
@@ -16379,7 +16400,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
         <v>72</v>
       </c>
@@ -16602,7 +16623,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
         <v>74</v>
       </c>
@@ -16715,7 +16736,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
         <v>75</v>
       </c>
@@ -16828,7 +16849,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
         <v>76</v>
       </c>
@@ -16974,7 +16995,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
         <v>77</v>
       </c>
@@ -17090,7 +17111,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
         <v>78</v>
       </c>
@@ -17203,7 +17224,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
         <v>79</v>
       </c>
@@ -17319,7 +17340,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
         <v>80</v>
       </c>
@@ -17545,7 +17566,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
         <v>82</v>
       </c>
@@ -17694,7 +17715,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
         <v>83</v>
       </c>
@@ -17831,7 +17852,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
         <v>84</v>
       </c>
@@ -17947,7 +17968,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
         <v>85</v>
       </c>
@@ -18310,7 +18331,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
         <v>88</v>
       </c>
@@ -18453,7 +18474,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
         <v>89</v>
       </c>
@@ -18569,7 +18590,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
         <v>90</v>
       </c>
@@ -18679,7 +18700,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
         <v>91</v>
       </c>
@@ -18822,7 +18843,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
         <v>92</v>
       </c>
@@ -18935,7 +18956,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
         <v>93</v>
       </c>
@@ -19182,7 +19203,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
         <v>95</v>
       </c>
@@ -19295,7 +19316,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="n">
         <v>96</v>
       </c>
@@ -19408,7 +19429,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="n">
         <v>97</v>
       </c>
@@ -19634,7 +19655,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="n">
         <v>99</v>
       </c>
@@ -19747,7 +19768,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="n">
         <v>100</v>
       </c>
@@ -19860,7 +19881,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="n">
         <v>101</v>
       </c>
@@ -19970,7 +19991,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="n">
         <v>102</v>
       </c>
@@ -20083,7 +20104,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="n">
         <v>103</v>
       </c>
@@ -20229,7 +20250,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="n">
         <v>104</v>
       </c>
@@ -20372,7 +20393,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="n">
         <v>105</v>
       </c>
@@ -20485,7 +20506,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="n">
         <v>106</v>
       </c>
@@ -20601,7 +20622,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
         <v>107</v>
       </c>
@@ -20714,7 +20735,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
         <v>108</v>
       </c>
@@ -20827,7 +20848,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
         <v>109</v>
       </c>
@@ -20949,7 +20970,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
         <v>110</v>
       </c>
@@ -21059,7 +21080,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
         <v>111</v>
       </c>
@@ -21172,7 +21193,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
         <v>112</v>
       </c>
@@ -21285,7 +21306,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
         <v>113</v>
       </c>
@@ -21428,7 +21449,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
         <v>114</v>
       </c>
@@ -21681,7 +21702,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
         <v>116</v>
       </c>
@@ -21910,7 +21931,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="n">
         <v>118</v>
       </c>
@@ -22053,7 +22074,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="n">
         <v>119</v>
       </c>
@@ -22297,7 +22318,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="n">
         <v>121</v>
       </c>
@@ -22541,7 +22562,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="n">
         <v>123</v>
       </c>
@@ -23449,7 +23470,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="n">
         <v>130</v>
       </c>
@@ -23565,7 +23586,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
         <v>131</v>
       </c>
@@ -23681,7 +23702,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="n">
         <v>132</v>
       </c>
@@ -23794,7 +23815,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
         <v>133</v>
       </c>
@@ -23937,7 +23958,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
         <v>134</v>
       </c>
@@ -24050,7 +24071,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="n">
         <v>135</v>
       </c>
@@ -24166,7 +24187,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="n">
         <v>136</v>
       </c>
@@ -24279,7 +24300,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="n">
         <v>137</v>
       </c>
@@ -24413,7 +24434,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="n">
         <v>138</v>
       </c>
@@ -24639,7 +24660,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="n">
         <v>140</v>
       </c>
@@ -25017,7 +25038,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="n">
         <v>143</v>
       </c>
@@ -25261,7 +25282,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="n">
         <v>145</v>
       </c>
@@ -25725,7 +25746,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
         <v>149</v>
       </c>
@@ -25838,7 +25859,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="n">
         <v>150</v>
       </c>
@@ -25981,7 +26002,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="n">
         <v>151</v>
       </c>
@@ -26234,7 +26255,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="n">
         <v>153</v>
       </c>
@@ -26460,7 +26481,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
         <v>155</v>
       </c>
@@ -26576,7 +26597,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
         <v>156</v>
       </c>
@@ -26689,7 +26710,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
         <v>157</v>
       </c>
@@ -26811,7 +26832,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
         <v>158</v>
       </c>
@@ -26927,7 +26948,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="n">
         <v>159</v>
       </c>
@@ -27049,7 +27070,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="n">
         <v>160</v>
       </c>
@@ -27186,7 +27207,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
         <v>161</v>
       </c>
@@ -27302,7 +27323,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
         <v>162</v>
       </c>
@@ -27418,7 +27439,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="n">
         <v>163</v>
       </c>
@@ -27561,7 +27582,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="n">
         <v>164</v>
       </c>
@@ -27680,7 +27701,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
         <v>165</v>
       </c>
@@ -27796,7 +27817,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
         <v>166</v>
       </c>
@@ -27909,7 +27930,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="n">
         <v>167</v>
       </c>
@@ -28564,7 +28585,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
         <v>172</v>
       </c>
@@ -28817,7 +28838,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="n">
         <v>174</v>
       </c>
@@ -28939,7 +28960,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="n">
         <v>175</v>
       </c>
@@ -29284,7 +29305,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="n">
         <v>178</v>
       </c>
@@ -29397,7 +29418,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
         <v>179</v>
       </c>
@@ -29513,7 +29534,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
         <v>180</v>
       </c>
@@ -29626,7 +29647,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
         <v>181</v>
       </c>
@@ -29739,7 +29760,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="n">
         <v>182</v>
       </c>
@@ -29882,7 +29903,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="n">
         <v>183</v>
       </c>
@@ -30025,7 +30046,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="n">
         <v>184</v>
       </c>
@@ -30141,7 +30162,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
         <v>185</v>
       </c>
@@ -30287,7 +30308,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="n">
         <v>186</v>
       </c>
@@ -30400,7 +30421,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="n">
         <v>187</v>
       </c>
@@ -30513,7 +30534,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="n">
         <v>188</v>
       </c>
@@ -30626,7 +30647,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
         <v>189</v>
       </c>
@@ -30742,7 +30763,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="n">
         <v>190</v>
       </c>
@@ -30968,7 +30989,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="n">
         <v>192</v>
       </c>
@@ -31111,7 +31132,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="n">
         <v>193</v>
       </c>
@@ -31224,7 +31245,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="n">
         <v>194</v>
       </c>
@@ -31337,7 +31358,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="n">
         <v>195</v>
       </c>
@@ -31453,7 +31474,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="n">
         <v>196</v>
       </c>
@@ -31569,7 +31590,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="n">
         <v>197</v>
       </c>
@@ -31685,7 +31706,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
         <v>198</v>
       </c>
@@ -31801,7 +31822,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
         <v>199</v>
       </c>
@@ -31944,7 +31965,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
         <v>200</v>
       </c>
@@ -32057,7 +32078,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="n">
         <v>201</v>
       </c>
@@ -32280,7 +32301,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="n">
         <v>203</v>
       </c>
@@ -32393,7 +32414,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="n">
         <v>204</v>
       </c>
@@ -32509,7 +32530,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="n">
         <v>205</v>
       </c>
@@ -32622,7 +32643,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="n">
         <v>206</v>
       </c>
@@ -33128,7 +33149,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="n">
         <v>210</v>
       </c>
@@ -33244,7 +33265,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="n">
         <v>211</v>
       </c>
@@ -33357,7 +33378,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="n">
         <v>212</v>
       </c>
@@ -33470,7 +33491,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="n">
         <v>213</v>
       </c>
@@ -33976,7 +33997,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="n">
         <v>217</v>
       </c>
@@ -34089,7 +34110,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="n">
         <v>218</v>
       </c>
@@ -34351,7 +34372,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="n">
         <v>220</v>
       </c>
@@ -34497,7 +34518,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="n">
         <v>221</v>
       </c>
@@ -34607,7 +34628,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="n">
         <v>222</v>
       </c>
@@ -34723,7 +34744,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="n">
         <v>223</v>
       </c>
@@ -34839,7 +34860,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="n">
         <v>224</v>
       </c>
@@ -34952,7 +34973,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="n">
         <v>225</v>
       </c>
@@ -35095,7 +35116,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="n">
         <v>226</v>
       </c>
@@ -35208,7 +35229,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="n">
         <v>227</v>
       </c>
@@ -35321,7 +35342,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="n">
         <v>228</v>
       </c>
@@ -35434,7 +35455,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="n">
         <v>229</v>
       </c>
@@ -35550,7 +35571,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="n">
         <v>230</v>
       </c>
@@ -35666,7 +35687,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="n">
         <v>231</v>
       </c>
@@ -35779,7 +35800,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="n">
         <v>232</v>
       </c>
@@ -36032,7 +36053,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="n">
         <v>234</v>
       </c>
@@ -36148,7 +36169,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="n">
         <v>235</v>
       </c>
@@ -36294,7 +36315,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="n">
         <v>236</v>
       </c>
@@ -36517,7 +36538,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="n">
         <v>238</v>
       </c>
@@ -36636,7 +36657,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="n">
         <v>239</v>
       </c>
@@ -36749,7 +36770,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="n">
         <v>240</v>
       </c>
@@ -36865,7 +36886,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="n">
         <v>241</v>
       </c>
@@ -37356,7 +37377,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="n">
         <v>245</v>
       </c>
@@ -37764,7 +37785,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="n">
         <v>248</v>
       </c>
@@ -37877,7 +37898,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="n">
         <v>249</v>
       </c>
@@ -37993,7 +38014,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="n">
         <v>250</v>
       </c>
@@ -38109,7 +38130,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="n">
         <v>251</v>
       </c>
@@ -38225,7 +38246,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="n">
         <v>252</v>
       </c>
@@ -38338,7 +38359,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="n">
         <v>253</v>
       </c>
@@ -38451,7 +38472,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="n">
         <v>254</v>
       </c>
@@ -38573,7 +38594,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="n">
         <v>255</v>
       </c>
@@ -38689,7 +38710,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="n">
         <v>256</v>
       </c>
@@ -39076,7 +39097,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="n">
         <v>259</v>
       </c>
@@ -39192,7 +39213,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="n">
         <v>260</v>
       </c>
@@ -39209,7 +39230,7 @@
         <v>44340</v>
       </c>
       <c r="F267" s="11" t="n">
-        <v>0.374305555555555</v>
+        <v>0.374305555555556</v>
       </c>
       <c r="G267" s="1" t="s">
         <v>85</v>
@@ -39278,7 +39299,7 @@
         <v>44340</v>
       </c>
       <c r="AM267" s="11" t="n">
-        <v>0.374305555555555</v>
+        <v>0.374305555555556</v>
       </c>
       <c r="AN267" s="1" t="s">
         <v>104</v>
@@ -39305,7 +39326,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="n">
         <v>261</v>
       </c>
@@ -39674,7 +39695,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="n">
         <v>264</v>
       </c>
@@ -39811,7 +39832,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="n">
         <v>265</v>
       </c>
@@ -39924,7 +39945,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="n">
         <v>266</v>
       </c>
@@ -40037,7 +40058,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="n">
         <v>267</v>
       </c>
@@ -40153,7 +40174,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="n">
         <v>268</v>
       </c>
@@ -40266,7 +40287,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="n">
         <v>269</v>
       </c>
@@ -40409,7 +40430,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="n">
         <v>270</v>
       </c>
@@ -40531,7 +40552,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="n">
         <v>271</v>
       </c>
@@ -40647,7 +40668,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="n">
         <v>272</v>
       </c>
@@ -40763,7 +40784,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="n">
         <v>273</v>
       </c>
@@ -40879,7 +40900,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="n">
         <v>274</v>
       </c>
@@ -40995,7 +41016,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="n">
         <v>275</v>
       </c>
@@ -41105,7 +41126,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="n">
         <v>276</v>
       </c>
@@ -41593,7 +41614,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="n">
         <v>280</v>
       </c>
@@ -42075,7 +42096,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="n">
         <v>284</v>
       </c>
@@ -42188,7 +42209,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="n">
         <v>285</v>
       </c>
@@ -42307,7 +42328,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="n">
         <v>286</v>
       </c>
@@ -42420,7 +42441,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="n">
         <v>287</v>
       </c>
@@ -42533,7 +42554,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="n">
         <v>288</v>
       </c>
@@ -42646,7 +42667,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="n">
         <v>289</v>
       </c>
@@ -42756,7 +42777,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="n">
         <v>290</v>
       </c>
@@ -42899,7 +42920,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="n">
         <v>291</v>
       </c>
@@ -43015,7 +43036,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="n">
         <v>292</v>
       </c>
@@ -43372,7 +43393,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="n">
         <v>295</v>
       </c>
@@ -43515,7 +43536,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="n">
         <v>296</v>
       </c>
@@ -43631,7 +43652,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="n">
         <v>297</v>
       </c>
@@ -43750,7 +43771,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="n">
         <v>298</v>
       </c>
@@ -43866,7 +43887,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="n">
         <v>299</v>
       </c>
@@ -43979,7 +44000,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="n">
         <v>300</v>
       </c>
@@ -44092,7 +44113,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="n">
         <v>301</v>
       </c>
@@ -44205,7 +44226,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="n">
         <v>302</v>
       </c>
@@ -44321,7 +44342,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="n">
         <v>303</v>
       </c>
@@ -44467,7 +44488,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="n">
         <v>304</v>
       </c>
@@ -44580,7 +44601,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="n">
         <v>305</v>
       </c>
@@ -44693,7 +44714,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="n">
         <v>306</v>
       </c>
@@ -44809,7 +44830,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="n">
         <v>307</v>
       </c>
@@ -44922,7 +44943,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="n">
         <v>308</v>
       </c>
@@ -45276,7 +45297,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="n">
         <v>311</v>
       </c>
@@ -45389,7 +45410,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="n">
         <v>312</v>
       </c>
@@ -45499,7 +45520,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="n">
         <v>313</v>
       </c>
@@ -45612,7 +45633,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="n">
         <v>314</v>
       </c>
@@ -46148,7 +46169,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="n">
         <v>318</v>
       </c>
@@ -46404,7 +46425,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="n">
         <v>320</v>
       </c>
@@ -46520,7 +46541,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="n">
         <v>321</v>
       </c>
@@ -46636,7 +46657,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="n">
         <v>322</v>
       </c>
@@ -46883,7 +46904,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="n">
         <v>324</v>
       </c>
@@ -46996,7 +47017,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="n">
         <v>325</v>
       </c>
@@ -47112,7 +47133,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="n">
         <v>326</v>
       </c>
@@ -47225,7 +47246,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="n">
         <v>327</v>
       </c>
@@ -47355,7 +47376,7 @@
         <v>44344</v>
       </c>
       <c r="F335" s="11" t="n">
-        <v>0.743055555555555</v>
+        <v>0.743055555555556</v>
       </c>
       <c r="G335" s="1" t="s">
         <v>141</v>
@@ -47421,7 +47442,7 @@
         <v>44344</v>
       </c>
       <c r="AM335" s="11" t="n">
-        <v>0.743055555555555</v>
+        <v>0.743055555555556</v>
       </c>
       <c r="AN335" s="1" t="s">
         <v>104</v>
@@ -47448,7 +47469,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="n">
         <v>329</v>
       </c>
@@ -47561,7 +47582,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="n">
         <v>330</v>
       </c>
@@ -47677,7 +47698,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="n">
         <v>331</v>
       </c>
@@ -47793,7 +47814,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="n">
         <v>332</v>
       </c>
@@ -47906,7 +47927,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="n">
         <v>333</v>
       </c>
@@ -48040,7 +48061,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="n">
         <v>334</v>
       </c>
@@ -48174,7 +48195,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="n">
         <v>335</v>
       </c>
@@ -48287,7 +48308,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="n">
         <v>336</v>
       </c>
@@ -48403,7 +48424,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="n">
         <v>337</v>
       </c>
@@ -48680,7 +48701,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="1" t="n">
         <v>339</v>
       </c>
@@ -48793,7 +48814,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="1" t="n">
         <v>340</v>
       </c>
@@ -48936,7 +48957,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="n">
         <v>341</v>
       </c>
@@ -49049,7 +49070,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="1" t="n">
         <v>342</v>
       </c>
@@ -49308,7 +49329,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="1" t="n">
         <v>344</v>
       </c>
@@ -49421,7 +49442,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="1" t="n">
         <v>345</v>
       </c>
@@ -49562,6 +49583,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="G7:G352">
+    <filterColumn colId="0">
+      <customFilters and="true">
+        <customFilter operator="equal" val="JURIDICA"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:F6"/>

</xml_diff>